<commit_message>
ICDC all breed test cases updated
</commit_message>
<xml_diff>
--- a/InputFiles/TC37_Canine_Filter_Breed-ParsonRussTerr.xlsx
+++ b/InputFiles/TC37_Canine_Filter_Breed-ParsonRussTerr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF674876-44E5-4E0A-8EFD-D93F6D900CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E3EA4-D821-437E-B19A-9A9FAA86A6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -117,8 +117,7 @@
         coalesce(f.file_description, '') AS `Description`,
         coalesce(f.file_format, '') AS `Format`,
         coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed , 
+        coalesce(c.case_id, '') AS `Case ID`, 
         coalesce(diag.disease_term,'') AS Diagnosis , 
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
@@ -557,7 +556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>